<commit_message>
cleared bugs and pending task
</commit_message>
<xml_diff>
--- a/views/import/product.xlsx
+++ b/views/import/product.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -68,6 +68,9 @@
   </si>
   <si>
     <t xml:space="preserve">eightdaysecuritydeposit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">suggestedProduct</t>
   </si>
   <si>
     <t xml:space="preserve">images</t>
@@ -80,7 +83,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -108,6 +111,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -152,12 +161,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -178,15 +191,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q1"/>
+  <dimension ref="A1:R1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R1" activeCellId="0" sqref="R:R"/>
+      <selection pane="topLeft" activeCell="Q1" activeCellId="0" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="15" min="2" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="27"/>
+    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -238,8 +254,11 @@
       <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="2" t="s">
         <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>